<commit_message>
Added a method that retrieves all teachers lessons
</commit_message>
<xml_diff>
--- a/Files/activePlans.xlsx
+++ b/Files/activePlans.xlsx
@@ -12,1332 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="1034">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="594">
   <si>
     <t>Name</t>
   </si>
   <si>
     <t>Link</t>
-  </si>
-  <si>
-    <t>AiR/NW/2sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=97778</t>
-  </si>
-  <si>
-    <t>AiR/NW/2sem/1gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=151300</t>
-  </si>
-  <si>
-    <t>AiR/NW/4sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=97781</t>
-  </si>
-  <si>
-    <t>AiR/NW/6sem/1gr/a/MiR</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=97783</t>
-  </si>
-  <si>
-    <t>AiR/NW/6sem/1gr/b/MiR</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=151317</t>
-  </si>
-  <si>
-    <t>AiR/NW/8sem/1gr/a/MiR</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=142125</t>
-  </si>
-  <si>
-    <t>AiR/S/2sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12340</t>
-  </si>
-  <si>
-    <t>AiR/S/2sem/1gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12341</t>
-  </si>
-  <si>
-    <t>AiR/S/2sem/1gr/c</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=154829</t>
-  </si>
-  <si>
-    <t>AiR/S/4sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12348</t>
-  </si>
-  <si>
-    <t>AiR/S/4sem/1gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12349</t>
-  </si>
-  <si>
-    <t>AiR/S/6sem/1gr/a/MiR</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=151201</t>
-  </si>
-  <si>
-    <t>AiR/S/6sem/1gr/b/MiR</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=151202</t>
-  </si>
-  <si>
-    <t>Analit/NZ/2sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=66973</t>
-  </si>
-  <si>
-    <t>Analit/NZ/2sem/1gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=137531</t>
-  </si>
-  <si>
-    <t>Analit/NZ/4sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=85760</t>
-  </si>
-  <si>
-    <t>Analit/NZ/4sem/1gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=150609</t>
-  </si>
-  <si>
-    <t>Analit/NZ/6sem 1</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=85762</t>
-  </si>
-  <si>
-    <t>Analit/S/2sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=66984</t>
-  </si>
-  <si>
-    <t>Analit/S/2sem/1gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=66985</t>
-  </si>
-  <si>
-    <t>Analit/S/4sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=114469</t>
-  </si>
-  <si>
-    <t>Analit/S/4sem/1gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=137255</t>
-  </si>
-  <si>
-    <t>Analit/S/6sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=90983</t>
-  </si>
-  <si>
-    <t>Analit/S/6sem/1gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=145587</t>
-  </si>
-  <si>
-    <t>Bud/S/IIst/1sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=74834</t>
-  </si>
-  <si>
-    <t>Bud/S/Ist/2sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12825</t>
-  </si>
-  <si>
-    <t>Bud/S/Ist/2sem/1gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=71562</t>
-  </si>
-  <si>
-    <t>Bud/S/Ist/4sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=16772</t>
-  </si>
-  <si>
-    <t>Bud/S/Ist/4sem/1gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=127356</t>
-  </si>
-  <si>
-    <t>Bud/S/Ist/6sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=23345</t>
-  </si>
-  <si>
-    <t>Bud/S/Ist/6sem/1gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=145144</t>
-  </si>
-  <si>
-    <t>EP/NW/2sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=142129</t>
-  </si>
-  <si>
-    <t>EP/NW/4sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=127948</t>
-  </si>
-  <si>
-    <t>EP/NW/6sem/1gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=139918</t>
-  </si>
-  <si>
-    <t>EP/S/2sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=123648</t>
-  </si>
-  <si>
-    <t>EP/S/4sem/1gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=124693</t>
-  </si>
-  <si>
-    <t>EP/S/6sem/1gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=141067</t>
-  </si>
-  <si>
-    <t>Erasmus/WBMiI/sem_2</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=142130</t>
-  </si>
-  <si>
-    <t>Fil ang/S/IIst/2sem/1gr/naucz</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=145146</t>
-  </si>
-  <si>
-    <t>Fil ang/S/IIst/2sem/2gr/tłumacz</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=97004</t>
-  </si>
-  <si>
-    <t>Fil ang/S/Ist/2sem/1gr 1</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=59783</t>
-  </si>
-  <si>
-    <t>Fil ang/S/Ist/2sem/2gr 1</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=59782</t>
-  </si>
-  <si>
-    <t>Fil ang/S/Ist/2sem/3gr 1</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=59781</t>
-  </si>
-  <si>
-    <t>Fil ang/S/Ist/2sem/4gr 1</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=145145</t>
-  </si>
-  <si>
-    <t>Fil ang/S/Ist/4sem/1gr/a/naucz</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12540</t>
-  </si>
-  <si>
-    <t>Fil ang/S/Ist/4sem/2gr/a/TzAJB</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=152013</t>
-  </si>
-  <si>
-    <t>Fil ang/S/Ist/4sem/2gr/b/TzAJB</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=152014</t>
-  </si>
-  <si>
-    <t>Fil ang/S/Ist/4sem/3gr/TNTwP 1</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=152016</t>
-  </si>
-  <si>
-    <t>Fil ang/S/Ist/6sem/1gr/a/Naucz</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12545</t>
-  </si>
-  <si>
-    <t>Fil ang/S/Ist/6sem/2gr/a/TzAJB</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12547</t>
-  </si>
-  <si>
-    <t>Fil ang/S/Ist/6sem/2gr/b/TzAJB</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=84689</t>
-  </si>
-  <si>
-    <t>Fil hisz/S/IIst/4sem/1gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=145141</t>
-  </si>
-  <si>
-    <t>Fil hisz/S/Ist/2sem/1gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12517</t>
-  </si>
-  <si>
-    <t>Fil hisz/S/Ist/2sem/2gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12519</t>
-  </si>
-  <si>
-    <t>Fil hisz/S/Ist/4sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12521</t>
-  </si>
-  <si>
-    <t>Fil hisz/S/Ist/4sem/1gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=97352</t>
-  </si>
-  <si>
-    <t>Fil hisz/S/Ist/6sem/1gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12523</t>
-  </si>
-  <si>
-    <t>Fil pol/S/IIst/4sem/1gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12572</t>
-  </si>
-  <si>
-    <t>Fil pol/S/Ist/2sem/1gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12555</t>
-  </si>
-  <si>
-    <t>Fil pol/S/Ist/4sem/1gr/nau 1</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=92070</t>
-  </si>
-  <si>
-    <t>Fil pol/S/Ist/6sem/1gr/nau 1</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=98570</t>
-  </si>
-  <si>
-    <t>Inf/NZ/IIst/2sem/1gr/a/TTO</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=136941</t>
-  </si>
-  <si>
-    <t>Inf/NZ/IIst/2sem/1gr/b/SI</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=140985</t>
-  </si>
-  <si>
-    <t>Inf/NZ/Ist/2sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12150</t>
-  </si>
-  <si>
-    <t>Inf/NZ/Ist/2sem/1gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=61137</t>
-  </si>
-  <si>
-    <t>Inf/NZ/Ist/2sem/2gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=136936</t>
-  </si>
-  <si>
-    <t>Inf/NZ/Ist/2sem/2gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=140980</t>
-  </si>
-  <si>
-    <t>Inf/NZ/Ist/4sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12153</t>
-  </si>
-  <si>
-    <t>Inf/NZ/Ist/4sem/1gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=136935</t>
-  </si>
-  <si>
-    <t>Inf/NZ/Ist/4sem/2gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=136934</t>
-  </si>
-  <si>
-    <t>Inf/NZ/Ist/6sem/1gr/a/IO</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=18739</t>
-  </si>
-  <si>
-    <t>Inf/NZ/Ist/6sem/1gr/b/IO</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=136937</t>
-  </si>
-  <si>
-    <t>Inf/NZ/Ist/6sem/2gr/a/SKiBS</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=136940</t>
-  </si>
-  <si>
-    <t>Inf/NZ/Ist/6sem/2gr/b/SKiBS</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=150382</t>
-  </si>
-  <si>
-    <t>Inf/S/IIst/1sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=128459</t>
-  </si>
-  <si>
-    <t>Inf/S/IIst/1sem/1gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=136969</t>
-  </si>
-  <si>
-    <t>Inf/S/IIst/3sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=136967</t>
-  </si>
-  <si>
-    <t>Inf/S/IIst/3sem/1gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=136968</t>
-  </si>
-  <si>
-    <t>Inf/S/Ist/2sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12633</t>
-  </si>
-  <si>
-    <t>Inf/S/Ist/2sem/1gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12634</t>
-  </si>
-  <si>
-    <t>Inf/S/Ist/2sem/2gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12637</t>
-  </si>
-  <si>
-    <t>Inf/S/Ist/2sem/2gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=142123</t>
-  </si>
-  <si>
-    <t>Inf/S/Ist/2sem/3gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=126070</t>
-  </si>
-  <si>
-    <t>Inf/S/Ist/2sem/3gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=129984</t>
-  </si>
-  <si>
-    <t>Inf/S/Ist/4sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12646</t>
-  </si>
-  <si>
-    <t>Inf/S/Ist/4sem/1gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12647</t>
-  </si>
-  <si>
-    <t>Inf/S/Ist/4sem/2gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=99396</t>
-  </si>
-  <si>
-    <t>Inf/S/Ist/4sem/2gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=142131</t>
-  </si>
-  <si>
-    <t>Inf/S/Ist/4sem/3gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=136966</t>
-  </si>
-  <si>
-    <t>Inf/S/Ist/4sem/3gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=151659</t>
-  </si>
-  <si>
-    <t>Inf/S/Ist/6sem/1gr/a/IO</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12652</t>
-  </si>
-  <si>
-    <t>Inf/S/Ist/6sem/1gr/b/IO</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12653</t>
-  </si>
-  <si>
-    <t>Inf/S/Ist/6sem/2gr/a/IO</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=61023</t>
-  </si>
-  <si>
-    <t>Inf/S/Ist/6sem/2gr/b/IO</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=126134</t>
-  </si>
-  <si>
-    <t>Inf/S/Ist/6sem/3gr/a/IO</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=151714</t>
-  </si>
-  <si>
-    <t>Inż mat/S/IIst/1sem 1</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=94624</t>
-  </si>
-  <si>
-    <t>Inż mat/S/Ist/4sem/1gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=142140</t>
-  </si>
-  <si>
-    <t>Inż śr/S/IIst/1sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=25690</t>
-  </si>
-  <si>
-    <t>Inż śr/S/IIst/3sem/1gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=25699</t>
-  </si>
-  <si>
-    <t>Inż śr/S/Ist/2sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12740</t>
-  </si>
-  <si>
-    <t>Inż śr/S/Ist/2sem/1gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=152030</t>
-  </si>
-  <si>
-    <t>Inż śr/S/Ist/6sem/1gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=25683</t>
-  </si>
-  <si>
-    <t>Kom int/S/2sem/1gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=133552</t>
-  </si>
-  <si>
-    <t>Kom int/S/2sem/2gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=135845</t>
-  </si>
-  <si>
-    <t>Kom int/S/2sem/3gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=154998</t>
-  </si>
-  <si>
-    <t>Kom int/S/4sem/1gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=135848</t>
-  </si>
-  <si>
-    <t>Kom int/S/4sem/2gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=135849</t>
-  </si>
-  <si>
-    <t>MiBM/NW/Ist/2sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=142121</t>
-  </si>
-  <si>
-    <t>MiBM/NW/Ist/2sem/1gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=141076</t>
-  </si>
-  <si>
-    <t>MiBM/NW/Ist/4sem/1gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12124</t>
-  </si>
-  <si>
-    <t>MiBM/NW/Ist/6sem/1gr/a/KWiW</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12126</t>
-  </si>
-  <si>
-    <t>MiBM/NW/Ist/8sem/1gr/a/KWiW</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12129</t>
-  </si>
-  <si>
-    <t>MiBM/S/IIst/1sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=142122</t>
-  </si>
-  <si>
-    <t>MiBM/S/IIst/3sem/1gr/PiTD3D</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=142104</t>
-  </si>
-  <si>
-    <t>MiBM/S/Ist/2sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=126632</t>
-  </si>
-  <si>
-    <t>MiBM/S/Ist/4sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12605</t>
-  </si>
-  <si>
-    <t>MiBM/S/Ist/6sem/1gr/a/KWKiW</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12613</t>
-  </si>
-  <si>
-    <t>Mt/S/IIst/1sem/1gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=141169</t>
-  </si>
-  <si>
-    <t>Mt/S/IIst/2sem/1gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=142145</t>
-  </si>
-  <si>
-    <t>Ochr śr/S/4sem/1gr/EŚ</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12733</t>
-  </si>
-  <si>
-    <t>Ped/S/4sem/1gr/PSiTP</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=114712</t>
-  </si>
-  <si>
-    <t>Ped/S/Ist/2sem/1gr 1</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12577</t>
-  </si>
-  <si>
-    <t>Ped/S/Ist/2sem/2gr 1</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=151978</t>
-  </si>
-  <si>
-    <t>Ped/S/Ist/4sem/1gr/R</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=151980</t>
-  </si>
-  <si>
-    <t>Ped/S/Ist/6sem/1gr/PSiTP 1</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=145147</t>
-  </si>
-  <si>
-    <t>Piel/NZ/IIst/2sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=26849</t>
-  </si>
-  <si>
-    <t>Piel/NZ/IIst/2sem/1gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=98643</t>
-  </si>
-  <si>
-    <t>Piel/NZ/IIst/4sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=36930</t>
-  </si>
-  <si>
-    <t>Piel/NZ/IIst/4sem/1gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=151507</t>
-  </si>
-  <si>
-    <t>Piel/S/IIst/2sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=29133</t>
-  </si>
-  <si>
-    <t>Piel/S/IIst/2sem/1gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=98644</t>
-  </si>
-  <si>
-    <t>Piel/S/IIst/4sem/1gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=39689</t>
-  </si>
-  <si>
-    <t>Piel/S/IIst/4sem/2gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=100885</t>
-  </si>
-  <si>
-    <t>Piel/S/Ist/2sem/1gr 1</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12694</t>
-  </si>
-  <si>
-    <t>Piel/S/Ist/2sem/2gr 1</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=100264</t>
-  </si>
-  <si>
-    <t>Piel/S/Ist/2sem/3gr 1</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=105351</t>
-  </si>
-  <si>
-    <t>Piel/S/Ist/2sem/4gr 1</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=141524</t>
-  </si>
-  <si>
-    <t>Piel/S/Ist/4sem/1gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=98672</t>
-  </si>
-  <si>
-    <t>Piel/S/Ist/4sem/2gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=100877</t>
-  </si>
-  <si>
-    <t>Piel/S/Ist/4sem/3gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=116611</t>
-  </si>
-  <si>
-    <t>Piel/S/Ist/6sem/1gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=152249</t>
-  </si>
-  <si>
-    <t>Piel/S/Ist/6sem/2gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=152252</t>
-  </si>
-  <si>
-    <t>Piel/S/Ist/6sem/3gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=152253</t>
-  </si>
-  <si>
-    <t>PPiW/S/JM/10sem 1</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=124697</t>
-  </si>
-  <si>
-    <t>PPiW/S/JM/2sem/1gr 1</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=95719</t>
-  </si>
-  <si>
-    <t>PPiW/S/JM/4sem/1gr 1</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=105266</t>
-  </si>
-  <si>
-    <t>PPiW/S/JM/6sem/1gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=105269</t>
-  </si>
-  <si>
-    <t>PPiW/S/JM/6sem/2gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=151981</t>
-  </si>
-  <si>
-    <t>PPiW/S/JM/8sem/1gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=123187</t>
-  </si>
-  <si>
-    <t>Rat/NZ/2sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=26851</t>
-  </si>
-  <si>
-    <t>Rat/NZ/2sem/1gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=37290</t>
-  </si>
-  <si>
-    <t>Rat/NZ/4sem/1gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=19073</t>
-  </si>
-  <si>
-    <t>Rat/S/2sem/1gr 1</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12698</t>
-  </si>
-  <si>
-    <t>Rat/S/2sem/2gr 1</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12819</t>
-  </si>
-  <si>
-    <t>Rat/S/4sem 1</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12699</t>
-  </si>
-  <si>
-    <t>Rat/S/6sem/1gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=152255</t>
-  </si>
-  <si>
-    <t>Rat/S/6sem/2gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=152256</t>
-  </si>
-  <si>
-    <t>Soc/S/4sem/1gr/a/KSiNM</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=115114</t>
-  </si>
-  <si>
-    <t>Soc/S/4sem/1gr/b/SOiZZ</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=150946</t>
-  </si>
-  <si>
-    <t>Soc/S/6sem/1gr/KSiNM</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=137311</t>
-  </si>
-  <si>
-    <t>Trans/NZ/IIst/2sem/1gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=85807</t>
-  </si>
-  <si>
-    <t>Trans/NZ/Ist/2sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12195</t>
-  </si>
-  <si>
-    <t>Trans/NZ/Ist/2sem/1gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=127194</t>
-  </si>
-  <si>
-    <t>Trans/NZ/Ist/4sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12200</t>
-  </si>
-  <si>
-    <t>Trans/NZ/Ist/6sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=25571</t>
-  </si>
-  <si>
-    <t>Trans/NZ/Ist/6sem/1gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=150627</t>
-  </si>
-  <si>
-    <t>Trans/NZ/Ist/8sem/1gr/EiBT</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=25573</t>
-  </si>
-  <si>
-    <t>Trans/S/IIst/1sem/1gr 1</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=86222</t>
-  </si>
-  <si>
-    <t>Trans/S/Ist/2sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12421</t>
-  </si>
-  <si>
-    <t>Trans/S/Ist/2sem/1gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12422</t>
-  </si>
-  <si>
-    <t>Trans/S/Ist/4sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12430</t>
-  </si>
-  <si>
-    <t>Trans/S/Ist/6sem/1gr/a/IST</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=19108</t>
-  </si>
-  <si>
-    <t>Trans/S/Ist/6sem/1gr/b/LiSK 1</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=137045</t>
-  </si>
-  <si>
-    <t>Tur/S/2sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=144981</t>
-  </si>
-  <si>
-    <t>Tur/S/2sem/1gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=145104</t>
-  </si>
-  <si>
-    <t>Tur/S/2sem/2gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=150451</t>
-  </si>
-  <si>
-    <t>Tur/S/2sem/2gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=150452</t>
-  </si>
-  <si>
-    <t>Zarz/NZ/IIst/2sem/1gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=85716</t>
-  </si>
-  <si>
-    <t>Zarz/NZ/Ist/2sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12207</t>
-  </si>
-  <si>
-    <t>Zarz/NZ/Ist/2sem/1gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=127378</t>
-  </si>
-  <si>
-    <t>Zarz/NZ/Ist/4sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12211</t>
-  </si>
-  <si>
-    <t>Zarz/NZ/Ist/4sem/1gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=127129</t>
-  </si>
-  <si>
-    <t>Zarz/NZ/Ist/6sem/1gr/a/ZLiJ</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=137451</t>
-  </si>
-  <si>
-    <t>Zarz/NZ/Ist/6sem/2gr/ZF 1</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12216</t>
-  </si>
-  <si>
-    <t>Zarz/S/IIst/2sem/1gr</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12473</t>
-  </si>
-  <si>
-    <t>Zarz/S/IIst/4sem/1gr/ZF 1</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12480</t>
-  </si>
-  <si>
-    <t>Zarz/S/IIst/4sem/2gr/ZwAiFO 1</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12481</t>
-  </si>
-  <si>
-    <t>Zarz/S/IIst/4sem/3gr/MLiJ 1</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=150863</t>
-  </si>
-  <si>
-    <t>Zarz/S/Ist/2sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12442</t>
-  </si>
-  <si>
-    <t>Zarz/S/Ist/2sem/1gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12443</t>
-  </si>
-  <si>
-    <t>Zarz/S/Ist/2sem/2gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12446</t>
-  </si>
-  <si>
-    <t>Zarz/S/Ist/2sem/2gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=127379</t>
-  </si>
-  <si>
-    <t>Zarz/S/Ist/2sem/3gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=150733</t>
-  </si>
-  <si>
-    <t>Zarz/S/Ist/2sem/3gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=150734</t>
-  </si>
-  <si>
-    <t>Zarz/S/Ist/4sem/1gr/ZF 1</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12456</t>
-  </si>
-  <si>
-    <t>Zarz/S/Ist/4sem/2gr/ZwAiFO 1</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12457</t>
-  </si>
-  <si>
-    <t>Zarz/S/Ist/4sem/3gr/ZLiJ 1</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=85061</t>
-  </si>
-  <si>
-    <t>Zarz/S/Ist/6sem/1gr/ZF 1</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=97080</t>
-  </si>
-  <si>
-    <t>Zarz/S/Ist/6sem/2gr/ZwAiFO 1</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12467</t>
-  </si>
-  <si>
-    <t>Zarz/S/Ist/6sem/3gr/ZLiJ 1</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12465</t>
-  </si>
-  <si>
-    <t>ZiIP/NZ/IIst/2sem/1gr/a/IZPrz</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=142124</t>
-  </si>
-  <si>
-    <t>ZiIP/NZ/IIst/2sem/1gr/b/IIPrz</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=140994</t>
-  </si>
-  <si>
-    <t>ZiIP/NZ/Ist/2sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12160</t>
-  </si>
-  <si>
-    <t>ZiIP/NZ/Ist/2sem/1gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12161</t>
-  </si>
-  <si>
-    <t>ZiIP/NZ/Ist/2sem/2gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=126203</t>
-  </si>
-  <si>
-    <t>ZiIP/NZ/Ist/2sem/2gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=151770</t>
-  </si>
-  <si>
-    <t>ZiIP/NZ/Ist/4sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12166</t>
-  </si>
-  <si>
-    <t>ZiIP/NZ/Ist/4sem/1gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12167</t>
-  </si>
-  <si>
-    <t>ZiIP/NZ/Ist/4sem/2gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=153575</t>
-  </si>
-  <si>
-    <t>ZiIP/NZ/Ist/6sem/1gr/a/IZP-PP</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12177</t>
-  </si>
-  <si>
-    <t>ZiIP/NZ/Ist/6sem/1gr/b/IZP-PP</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=142152</t>
-  </si>
-  <si>
-    <t>ZiIP/S/IIst/1sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12686</t>
-  </si>
-  <si>
-    <t>ZiIP/S/IIst/1sem/1gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=142263</t>
-  </si>
-  <si>
-    <t>ZiIP/S/IIst/3sem/1gr/IIPrz/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=136970</t>
-  </si>
-  <si>
-    <t>ZiIP/S/IIst/3sem/1gr/IIPrz/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=136971</t>
-  </si>
-  <si>
-    <t>ZiIP/S/Ist/2sem/1gr/a</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=25566</t>
-  </si>
-  <si>
-    <t>ZiIP/S/Ist/2sem/1gr/b</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12665</t>
-  </si>
-  <si>
-    <t>ZiIP/S/Ist/4sem/1gr 1</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=12670</t>
-  </si>
-  <si>
-    <t>ZiIP/S/Ist/6sem/1gr/a/IZS</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=142153</t>
-  </si>
-  <si>
-    <t>Zzl/S/2sem/1gr 1</t>
-  </si>
-  <si>
-    <t>plan.php?type=0&amp;id=145009</t>
   </si>
   <si>
     <t>A A</t>
@@ -3159,7 +1839,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B517"/>
+  <dimension ref="A1:B297"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5541,1766 +4221,6 @@
         <v>593</v>
       </c>
     </row>
-    <row r="298">
-      <c r="A298" s="0" t="s">
-        <v>594</v>
-      </c>
-      <c r="B298" s="0" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="299">
-      <c r="A299" s="0" t="s">
-        <v>596</v>
-      </c>
-      <c r="B299" s="0" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="300">
-      <c r="A300" s="0" t="s">
-        <v>598</v>
-      </c>
-      <c r="B300" s="0" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="301">
-      <c r="A301" s="0" t="s">
-        <v>600</v>
-      </c>
-      <c r="B301" s="0" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="302">
-      <c r="A302" s="0" t="s">
-        <v>602</v>
-      </c>
-      <c r="B302" s="0" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="303">
-      <c r="A303" s="0" t="s">
-        <v>604</v>
-      </c>
-      <c r="B303" s="0" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="304">
-      <c r="A304" s="0" t="s">
-        <v>606</v>
-      </c>
-      <c r="B304" s="0" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="305">
-      <c r="A305" s="0" t="s">
-        <v>608</v>
-      </c>
-      <c r="B305" s="0" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="306">
-      <c r="A306" s="0" t="s">
-        <v>610</v>
-      </c>
-      <c r="B306" s="0" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="307">
-      <c r="A307" s="0" t="s">
-        <v>612</v>
-      </c>
-      <c r="B307" s="0" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="308">
-      <c r="A308" s="0" t="s">
-        <v>614</v>
-      </c>
-      <c r="B308" s="0" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="309">
-      <c r="A309" s="0" t="s">
-        <v>616</v>
-      </c>
-      <c r="B309" s="0" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="310">
-      <c r="A310" s="0" t="s">
-        <v>618</v>
-      </c>
-      <c r="B310" s="0" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="311">
-      <c r="A311" s="0" t="s">
-        <v>620</v>
-      </c>
-      <c r="B311" s="0" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="312">
-      <c r="A312" s="0" t="s">
-        <v>622</v>
-      </c>
-      <c r="B312" s="0" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="313">
-      <c r="A313" s="0" t="s">
-        <v>624</v>
-      </c>
-      <c r="B313" s="0" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="314">
-      <c r="A314" s="0" t="s">
-        <v>626</v>
-      </c>
-      <c r="B314" s="0" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="315">
-      <c r="A315" s="0" t="s">
-        <v>628</v>
-      </c>
-      <c r="B315" s="0" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="316">
-      <c r="A316" s="0" t="s">
-        <v>630</v>
-      </c>
-      <c r="B316" s="0" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="317">
-      <c r="A317" s="0" t="s">
-        <v>632</v>
-      </c>
-      <c r="B317" s="0" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="318">
-      <c r="A318" s="0" t="s">
-        <v>634</v>
-      </c>
-      <c r="B318" s="0" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="319">
-      <c r="A319" s="0" t="s">
-        <v>636</v>
-      </c>
-      <c r="B319" s="0" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="320">
-      <c r="A320" s="0" t="s">
-        <v>638</v>
-      </c>
-      <c r="B320" s="0" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="321">
-      <c r="A321" s="0" t="s">
-        <v>640</v>
-      </c>
-      <c r="B321" s="0" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="322">
-      <c r="A322" s="0" t="s">
-        <v>642</v>
-      </c>
-      <c r="B322" s="0" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="323">
-      <c r="A323" s="0" t="s">
-        <v>644</v>
-      </c>
-      <c r="B323" s="0" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="324">
-      <c r="A324" s="0" t="s">
-        <v>646</v>
-      </c>
-      <c r="B324" s="0" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="325">
-      <c r="A325" s="0" t="s">
-        <v>648</v>
-      </c>
-      <c r="B325" s="0" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="326">
-      <c r="A326" s="0" t="s">
-        <v>650</v>
-      </c>
-      <c r="B326" s="0" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="327">
-      <c r="A327" s="0" t="s">
-        <v>652</v>
-      </c>
-      <c r="B327" s="0" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="328">
-      <c r="A328" s="0" t="s">
-        <v>654</v>
-      </c>
-      <c r="B328" s="0" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="329">
-      <c r="A329" s="0" t="s">
-        <v>656</v>
-      </c>
-      <c r="B329" s="0" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="330">
-      <c r="A330" s="0" t="s">
-        <v>658</v>
-      </c>
-      <c r="B330" s="0" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="331">
-      <c r="A331" s="0" t="s">
-        <v>660</v>
-      </c>
-      <c r="B331" s="0" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="332">
-      <c r="A332" s="0" t="s">
-        <v>662</v>
-      </c>
-      <c r="B332" s="0" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="333">
-      <c r="A333" s="0" t="s">
-        <v>664</v>
-      </c>
-      <c r="B333" s="0" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="334">
-      <c r="A334" s="0" t="s">
-        <v>666</v>
-      </c>
-      <c r="B334" s="0" t="s">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="335">
-      <c r="A335" s="0" t="s">
-        <v>668</v>
-      </c>
-      <c r="B335" s="0" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="336">
-      <c r="A336" s="0" t="s">
-        <v>670</v>
-      </c>
-      <c r="B336" s="0" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="337">
-      <c r="A337" s="0" t="s">
-        <v>672</v>
-      </c>
-      <c r="B337" s="0" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="338">
-      <c r="A338" s="0" t="s">
-        <v>674</v>
-      </c>
-      <c r="B338" s="0" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="339">
-      <c r="A339" s="0" t="s">
-        <v>676</v>
-      </c>
-      <c r="B339" s="0" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="340">
-      <c r="A340" s="0" t="s">
-        <v>678</v>
-      </c>
-      <c r="B340" s="0" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="341">
-      <c r="A341" s="0" t="s">
-        <v>680</v>
-      </c>
-      <c r="B341" s="0" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="342">
-      <c r="A342" s="0" t="s">
-        <v>682</v>
-      </c>
-      <c r="B342" s="0" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="343">
-      <c r="A343" s="0" t="s">
-        <v>684</v>
-      </c>
-      <c r="B343" s="0" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="344">
-      <c r="A344" s="0" t="s">
-        <v>686</v>
-      </c>
-      <c r="B344" s="0" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="345">
-      <c r="A345" s="0" t="s">
-        <v>688</v>
-      </c>
-      <c r="B345" s="0" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="346">
-      <c r="A346" s="0" t="s">
-        <v>690</v>
-      </c>
-      <c r="B346" s="0" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="347">
-      <c r="A347" s="0" t="s">
-        <v>692</v>
-      </c>
-      <c r="B347" s="0" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="348">
-      <c r="A348" s="0" t="s">
-        <v>694</v>
-      </c>
-      <c r="B348" s="0" t="s">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="349">
-      <c r="A349" s="0" t="s">
-        <v>696</v>
-      </c>
-      <c r="B349" s="0" t="s">
-        <v>697</v>
-      </c>
-    </row>
-    <row r="350">
-      <c r="A350" s="0" t="s">
-        <v>698</v>
-      </c>
-      <c r="B350" s="0" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="351">
-      <c r="A351" s="0" t="s">
-        <v>700</v>
-      </c>
-      <c r="B351" s="0" t="s">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="352">
-      <c r="A352" s="0" t="s">
-        <v>702</v>
-      </c>
-      <c r="B352" s="0" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="353">
-      <c r="A353" s="0" t="s">
-        <v>704</v>
-      </c>
-      <c r="B353" s="0" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="354">
-      <c r="A354" s="0" t="s">
-        <v>706</v>
-      </c>
-      <c r="B354" s="0" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="355">
-      <c r="A355" s="0" t="s">
-        <v>708</v>
-      </c>
-      <c r="B355" s="0" t="s">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="356">
-      <c r="A356" s="0" t="s">
-        <v>710</v>
-      </c>
-      <c r="B356" s="0" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="357">
-      <c r="A357" s="0" t="s">
-        <v>712</v>
-      </c>
-      <c r="B357" s="0" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="358">
-      <c r="A358" s="0" t="s">
-        <v>714</v>
-      </c>
-      <c r="B358" s="0" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="359">
-      <c r="A359" s="0" t="s">
-        <v>716</v>
-      </c>
-      <c r="B359" s="0" t="s">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="360">
-      <c r="A360" s="0" t="s">
-        <v>718</v>
-      </c>
-      <c r="B360" s="0" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="361">
-      <c r="A361" s="0" t="s">
-        <v>720</v>
-      </c>
-      <c r="B361" s="0" t="s">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="362">
-      <c r="A362" s="0" t="s">
-        <v>722</v>
-      </c>
-      <c r="B362" s="0" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="363">
-      <c r="A363" s="0" t="s">
-        <v>724</v>
-      </c>
-      <c r="B363" s="0" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="364">
-      <c r="A364" s="0" t="s">
-        <v>726</v>
-      </c>
-      <c r="B364" s="0" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="365">
-      <c r="A365" s="0" t="s">
-        <v>728</v>
-      </c>
-      <c r="B365" s="0" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="366">
-      <c r="A366" s="0" t="s">
-        <v>730</v>
-      </c>
-      <c r="B366" s="0" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="367">
-      <c r="A367" s="0" t="s">
-        <v>732</v>
-      </c>
-      <c r="B367" s="0" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="368">
-      <c r="A368" s="0" t="s">
-        <v>734</v>
-      </c>
-      <c r="B368" s="0" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="369">
-      <c r="A369" s="0" t="s">
-        <v>736</v>
-      </c>
-      <c r="B369" s="0" t="s">
-        <v>737</v>
-      </c>
-    </row>
-    <row r="370">
-      <c r="A370" s="0" t="s">
-        <v>738</v>
-      </c>
-      <c r="B370" s="0" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="371">
-      <c r="A371" s="0" t="s">
-        <v>740</v>
-      </c>
-      <c r="B371" s="0" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="372">
-      <c r="A372" s="0" t="s">
-        <v>742</v>
-      </c>
-      <c r="B372" s="0" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="373">
-      <c r="A373" s="0" t="s">
-        <v>744</v>
-      </c>
-      <c r="B373" s="0" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="374">
-      <c r="A374" s="0" t="s">
-        <v>746</v>
-      </c>
-      <c r="B374" s="0" t="s">
-        <v>747</v>
-      </c>
-    </row>
-    <row r="375">
-      <c r="A375" s="0" t="s">
-        <v>748</v>
-      </c>
-      <c r="B375" s="0" t="s">
-        <v>749</v>
-      </c>
-    </row>
-    <row r="376">
-      <c r="A376" s="0" t="s">
-        <v>750</v>
-      </c>
-      <c r="B376" s="0" t="s">
-        <v>751</v>
-      </c>
-    </row>
-    <row r="377">
-      <c r="A377" s="0" t="s">
-        <v>752</v>
-      </c>
-      <c r="B377" s="0" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="378">
-      <c r="A378" s="0" t="s">
-        <v>754</v>
-      </c>
-      <c r="B378" s="0" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="379">
-      <c r="A379" s="0" t="s">
-        <v>756</v>
-      </c>
-      <c r="B379" s="0" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="380">
-      <c r="A380" s="0" t="s">
-        <v>758</v>
-      </c>
-      <c r="B380" s="0" t="s">
-        <v>759</v>
-      </c>
-    </row>
-    <row r="381">
-      <c r="A381" s="0" t="s">
-        <v>760</v>
-      </c>
-      <c r="B381" s="0" t="s">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="382">
-      <c r="A382" s="0" t="s">
-        <v>762</v>
-      </c>
-      <c r="B382" s="0" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="383">
-      <c r="A383" s="0" t="s">
-        <v>764</v>
-      </c>
-      <c r="B383" s="0" t="s">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="384">
-      <c r="A384" s="0" t="s">
-        <v>766</v>
-      </c>
-      <c r="B384" s="0" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="385">
-      <c r="A385" s="0" t="s">
-        <v>768</v>
-      </c>
-      <c r="B385" s="0" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="386">
-      <c r="A386" s="0" t="s">
-        <v>770</v>
-      </c>
-      <c r="B386" s="0" t="s">
-        <v>771</v>
-      </c>
-    </row>
-    <row r="387">
-      <c r="A387" s="0" t="s">
-        <v>772</v>
-      </c>
-      <c r="B387" s="0" t="s">
-        <v>773</v>
-      </c>
-    </row>
-    <row r="388">
-      <c r="A388" s="0" t="s">
-        <v>774</v>
-      </c>
-      <c r="B388" s="0" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="389">
-      <c r="A389" s="0" t="s">
-        <v>776</v>
-      </c>
-      <c r="B389" s="0" t="s">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="390">
-      <c r="A390" s="0" t="s">
-        <v>778</v>
-      </c>
-      <c r="B390" s="0" t="s">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="391">
-      <c r="A391" s="0" t="s">
-        <v>780</v>
-      </c>
-      <c r="B391" s="0" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="392">
-      <c r="A392" s="0" t="s">
-        <v>782</v>
-      </c>
-      <c r="B392" s="0" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="393">
-      <c r="A393" s="0" t="s">
-        <v>784</v>
-      </c>
-      <c r="B393" s="0" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="394">
-      <c r="A394" s="0" t="s">
-        <v>786</v>
-      </c>
-      <c r="B394" s="0" t="s">
-        <v>787</v>
-      </c>
-    </row>
-    <row r="395">
-      <c r="A395" s="0" t="s">
-        <v>788</v>
-      </c>
-      <c r="B395" s="0" t="s">
-        <v>789</v>
-      </c>
-    </row>
-    <row r="396">
-      <c r="A396" s="0" t="s">
-        <v>790</v>
-      </c>
-      <c r="B396" s="0" t="s">
-        <v>791</v>
-      </c>
-    </row>
-    <row r="397">
-      <c r="A397" s="0" t="s">
-        <v>792</v>
-      </c>
-      <c r="B397" s="0" t="s">
-        <v>793</v>
-      </c>
-    </row>
-    <row r="398">
-      <c r="A398" s="0" t="s">
-        <v>794</v>
-      </c>
-      <c r="B398" s="0" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="399">
-      <c r="A399" s="0" t="s">
-        <v>796</v>
-      </c>
-      <c r="B399" s="0" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="400">
-      <c r="A400" s="0" t="s">
-        <v>798</v>
-      </c>
-      <c r="B400" s="0" t="s">
-        <v>799</v>
-      </c>
-    </row>
-    <row r="401">
-      <c r="A401" s="0" t="s">
-        <v>800</v>
-      </c>
-      <c r="B401" s="0" t="s">
-        <v>801</v>
-      </c>
-    </row>
-    <row r="402">
-      <c r="A402" s="0" t="s">
-        <v>802</v>
-      </c>
-      <c r="B402" s="0" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="403">
-      <c r="A403" s="0" t="s">
-        <v>804</v>
-      </c>
-      <c r="B403" s="0" t="s">
-        <v>805</v>
-      </c>
-    </row>
-    <row r="404">
-      <c r="A404" s="0" t="s">
-        <v>806</v>
-      </c>
-      <c r="B404" s="0" t="s">
-        <v>807</v>
-      </c>
-    </row>
-    <row r="405">
-      <c r="A405" s="0" t="s">
-        <v>808</v>
-      </c>
-      <c r="B405" s="0" t="s">
-        <v>809</v>
-      </c>
-    </row>
-    <row r="406">
-      <c r="A406" s="0" t="s">
-        <v>810</v>
-      </c>
-      <c r="B406" s="0" t="s">
-        <v>811</v>
-      </c>
-    </row>
-    <row r="407">
-      <c r="A407" s="0" t="s">
-        <v>812</v>
-      </c>
-      <c r="B407" s="0" t="s">
-        <v>813</v>
-      </c>
-    </row>
-    <row r="408">
-      <c r="A408" s="0" t="s">
-        <v>814</v>
-      </c>
-      <c r="B408" s="0" t="s">
-        <v>815</v>
-      </c>
-    </row>
-    <row r="409">
-      <c r="A409" s="0" t="s">
-        <v>816</v>
-      </c>
-      <c r="B409" s="0" t="s">
-        <v>817</v>
-      </c>
-    </row>
-    <row r="410">
-      <c r="A410" s="0" t="s">
-        <v>818</v>
-      </c>
-      <c r="B410" s="0" t="s">
-        <v>819</v>
-      </c>
-    </row>
-    <row r="411">
-      <c r="A411" s="0" t="s">
-        <v>820</v>
-      </c>
-      <c r="B411" s="0" t="s">
-        <v>821</v>
-      </c>
-    </row>
-    <row r="412">
-      <c r="A412" s="0" t="s">
-        <v>822</v>
-      </c>
-      <c r="B412" s="0" t="s">
-        <v>823</v>
-      </c>
-    </row>
-    <row r="413">
-      <c r="A413" s="0" t="s">
-        <v>824</v>
-      </c>
-      <c r="B413" s="0" t="s">
-        <v>825</v>
-      </c>
-    </row>
-    <row r="414">
-      <c r="A414" s="0" t="s">
-        <v>826</v>
-      </c>
-      <c r="B414" s="0" t="s">
-        <v>827</v>
-      </c>
-    </row>
-    <row r="415">
-      <c r="A415" s="0" t="s">
-        <v>828</v>
-      </c>
-      <c r="B415" s="0" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="416">
-      <c r="A416" s="0" t="s">
-        <v>830</v>
-      </c>
-      <c r="B416" s="0" t="s">
-        <v>831</v>
-      </c>
-    </row>
-    <row r="417">
-      <c r="A417" s="0" t="s">
-        <v>832</v>
-      </c>
-      <c r="B417" s="0" t="s">
-        <v>833</v>
-      </c>
-    </row>
-    <row r="418">
-      <c r="A418" s="0" t="s">
-        <v>834</v>
-      </c>
-      <c r="B418" s="0" t="s">
-        <v>835</v>
-      </c>
-    </row>
-    <row r="419">
-      <c r="A419" s="0" t="s">
-        <v>836</v>
-      </c>
-      <c r="B419" s="0" t="s">
-        <v>837</v>
-      </c>
-    </row>
-    <row r="420">
-      <c r="A420" s="0" t="s">
-        <v>838</v>
-      </c>
-      <c r="B420" s="0" t="s">
-        <v>839</v>
-      </c>
-    </row>
-    <row r="421">
-      <c r="A421" s="0" t="s">
-        <v>840</v>
-      </c>
-      <c r="B421" s="0" t="s">
-        <v>841</v>
-      </c>
-    </row>
-    <row r="422">
-      <c r="A422" s="0" t="s">
-        <v>842</v>
-      </c>
-      <c r="B422" s="0" t="s">
-        <v>843</v>
-      </c>
-    </row>
-    <row r="423">
-      <c r="A423" s="0" t="s">
-        <v>844</v>
-      </c>
-      <c r="B423" s="0" t="s">
-        <v>845</v>
-      </c>
-    </row>
-    <row r="424">
-      <c r="A424" s="0" t="s">
-        <v>846</v>
-      </c>
-      <c r="B424" s="0" t="s">
-        <v>847</v>
-      </c>
-    </row>
-    <row r="425">
-      <c r="A425" s="0" t="s">
-        <v>848</v>
-      </c>
-      <c r="B425" s="0" t="s">
-        <v>849</v>
-      </c>
-    </row>
-    <row r="426">
-      <c r="A426" s="0" t="s">
-        <v>850</v>
-      </c>
-      <c r="B426" s="0" t="s">
-        <v>851</v>
-      </c>
-    </row>
-    <row r="427">
-      <c r="A427" s="0" t="s">
-        <v>852</v>
-      </c>
-      <c r="B427" s="0" t="s">
-        <v>853</v>
-      </c>
-    </row>
-    <row r="428">
-      <c r="A428" s="0" t="s">
-        <v>854</v>
-      </c>
-      <c r="B428" s="0" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="429">
-      <c r="A429" s="0" t="s">
-        <v>856</v>
-      </c>
-      <c r="B429" s="0" t="s">
-        <v>857</v>
-      </c>
-    </row>
-    <row r="430">
-      <c r="A430" s="0" t="s">
-        <v>858</v>
-      </c>
-      <c r="B430" s="0" t="s">
-        <v>859</v>
-      </c>
-    </row>
-    <row r="431">
-      <c r="A431" s="0" t="s">
-        <v>860</v>
-      </c>
-      <c r="B431" s="0" t="s">
-        <v>861</v>
-      </c>
-    </row>
-    <row r="432">
-      <c r="A432" s="0" t="s">
-        <v>862</v>
-      </c>
-      <c r="B432" s="0" t="s">
-        <v>863</v>
-      </c>
-    </row>
-    <row r="433">
-      <c r="A433" s="0" t="s">
-        <v>864</v>
-      </c>
-      <c r="B433" s="0" t="s">
-        <v>865</v>
-      </c>
-    </row>
-    <row r="434">
-      <c r="A434" s="0" t="s">
-        <v>866</v>
-      </c>
-      <c r="B434" s="0" t="s">
-        <v>867</v>
-      </c>
-    </row>
-    <row r="435">
-      <c r="A435" s="0" t="s">
-        <v>868</v>
-      </c>
-      <c r="B435" s="0" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="436">
-      <c r="A436" s="0" t="s">
-        <v>870</v>
-      </c>
-      <c r="B436" s="0" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="437">
-      <c r="A437" s="0" t="s">
-        <v>872</v>
-      </c>
-      <c r="B437" s="0" t="s">
-        <v>873</v>
-      </c>
-    </row>
-    <row r="438">
-      <c r="A438" s="0" t="s">
-        <v>874</v>
-      </c>
-      <c r="B438" s="0" t="s">
-        <v>875</v>
-      </c>
-    </row>
-    <row r="439">
-      <c r="A439" s="0" t="s">
-        <v>876</v>
-      </c>
-      <c r="B439" s="0" t="s">
-        <v>877</v>
-      </c>
-    </row>
-    <row r="440">
-      <c r="A440" s="0" t="s">
-        <v>878</v>
-      </c>
-      <c r="B440" s="0" t="s">
-        <v>879</v>
-      </c>
-    </row>
-    <row r="441">
-      <c r="A441" s="0" t="s">
-        <v>880</v>
-      </c>
-      <c r="B441" s="0" t="s">
-        <v>881</v>
-      </c>
-    </row>
-    <row r="442">
-      <c r="A442" s="0" t="s">
-        <v>882</v>
-      </c>
-      <c r="B442" s="0" t="s">
-        <v>883</v>
-      </c>
-    </row>
-    <row r="443">
-      <c r="A443" s="0" t="s">
-        <v>884</v>
-      </c>
-      <c r="B443" s="0" t="s">
-        <v>885</v>
-      </c>
-    </row>
-    <row r="444">
-      <c r="A444" s="0" t="s">
-        <v>886</v>
-      </c>
-      <c r="B444" s="0" t="s">
-        <v>887</v>
-      </c>
-    </row>
-    <row r="445">
-      <c r="A445" s="0" t="s">
-        <v>888</v>
-      </c>
-      <c r="B445" s="0" t="s">
-        <v>889</v>
-      </c>
-    </row>
-    <row r="446">
-      <c r="A446" s="0" t="s">
-        <v>890</v>
-      </c>
-      <c r="B446" s="0" t="s">
-        <v>891</v>
-      </c>
-    </row>
-    <row r="447">
-      <c r="A447" s="0" t="s">
-        <v>892</v>
-      </c>
-      <c r="B447" s="0" t="s">
-        <v>893</v>
-      </c>
-    </row>
-    <row r="448">
-      <c r="A448" s="0" t="s">
-        <v>894</v>
-      </c>
-      <c r="B448" s="0" t="s">
-        <v>895</v>
-      </c>
-    </row>
-    <row r="449">
-      <c r="A449" s="0" t="s">
-        <v>896</v>
-      </c>
-      <c r="B449" s="0" t="s">
-        <v>897</v>
-      </c>
-    </row>
-    <row r="450">
-      <c r="A450" s="0" t="s">
-        <v>898</v>
-      </c>
-      <c r="B450" s="0" t="s">
-        <v>899</v>
-      </c>
-    </row>
-    <row r="451">
-      <c r="A451" s="0" t="s">
-        <v>900</v>
-      </c>
-      <c r="B451" s="0" t="s">
-        <v>901</v>
-      </c>
-    </row>
-    <row r="452">
-      <c r="A452" s="0" t="s">
-        <v>902</v>
-      </c>
-      <c r="B452" s="0" t="s">
-        <v>903</v>
-      </c>
-    </row>
-    <row r="453">
-      <c r="A453" s="0" t="s">
-        <v>904</v>
-      </c>
-      <c r="B453" s="0" t="s">
-        <v>905</v>
-      </c>
-    </row>
-    <row r="454">
-      <c r="A454" s="0" t="s">
-        <v>906</v>
-      </c>
-      <c r="B454" s="0" t="s">
-        <v>907</v>
-      </c>
-    </row>
-    <row r="455">
-      <c r="A455" s="0" t="s">
-        <v>908</v>
-      </c>
-      <c r="B455" s="0" t="s">
-        <v>909</v>
-      </c>
-    </row>
-    <row r="456">
-      <c r="A456" s="0" t="s">
-        <v>910</v>
-      </c>
-      <c r="B456" s="0" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="457">
-      <c r="A457" s="0" t="s">
-        <v>912</v>
-      </c>
-      <c r="B457" s="0" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="458">
-      <c r="A458" s="0" t="s">
-        <v>914</v>
-      </c>
-      <c r="B458" s="0" t="s">
-        <v>915</v>
-      </c>
-    </row>
-    <row r="459">
-      <c r="A459" s="0" t="s">
-        <v>916</v>
-      </c>
-      <c r="B459" s="0" t="s">
-        <v>917</v>
-      </c>
-    </row>
-    <row r="460">
-      <c r="A460" s="0" t="s">
-        <v>918</v>
-      </c>
-      <c r="B460" s="0" t="s">
-        <v>919</v>
-      </c>
-    </row>
-    <row r="461">
-      <c r="A461" s="0" t="s">
-        <v>920</v>
-      </c>
-      <c r="B461" s="0" t="s">
-        <v>921</v>
-      </c>
-    </row>
-    <row r="462">
-      <c r="A462" s="0" t="s">
-        <v>922</v>
-      </c>
-      <c r="B462" s="0" t="s">
-        <v>923</v>
-      </c>
-    </row>
-    <row r="463">
-      <c r="A463" s="0" t="s">
-        <v>924</v>
-      </c>
-      <c r="B463" s="0" t="s">
-        <v>925</v>
-      </c>
-    </row>
-    <row r="464">
-      <c r="A464" s="0" t="s">
-        <v>926</v>
-      </c>
-      <c r="B464" s="0" t="s">
-        <v>927</v>
-      </c>
-    </row>
-    <row r="465">
-      <c r="A465" s="0" t="s">
-        <v>928</v>
-      </c>
-      <c r="B465" s="0" t="s">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="466">
-      <c r="A466" s="0" t="s">
-        <v>930</v>
-      </c>
-      <c r="B466" s="0" t="s">
-        <v>931</v>
-      </c>
-    </row>
-    <row r="467">
-      <c r="A467" s="0" t="s">
-        <v>932</v>
-      </c>
-      <c r="B467" s="0" t="s">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="468">
-      <c r="A468" s="0" t="s">
-        <v>934</v>
-      </c>
-      <c r="B468" s="0" t="s">
-        <v>935</v>
-      </c>
-    </row>
-    <row r="469">
-      <c r="A469" s="0" t="s">
-        <v>936</v>
-      </c>
-      <c r="B469" s="0" t="s">
-        <v>937</v>
-      </c>
-    </row>
-    <row r="470">
-      <c r="A470" s="0" t="s">
-        <v>938</v>
-      </c>
-      <c r="B470" s="0" t="s">
-        <v>939</v>
-      </c>
-    </row>
-    <row r="471">
-      <c r="A471" s="0" t="s">
-        <v>940</v>
-      </c>
-      <c r="B471" s="0" t="s">
-        <v>941</v>
-      </c>
-    </row>
-    <row r="472">
-      <c r="A472" s="0" t="s">
-        <v>942</v>
-      </c>
-      <c r="B472" s="0" t="s">
-        <v>943</v>
-      </c>
-    </row>
-    <row r="473">
-      <c r="A473" s="0" t="s">
-        <v>944</v>
-      </c>
-      <c r="B473" s="0" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="474">
-      <c r="A474" s="0" t="s">
-        <v>946</v>
-      </c>
-      <c r="B474" s="0" t="s">
-        <v>947</v>
-      </c>
-    </row>
-    <row r="475">
-      <c r="A475" s="0" t="s">
-        <v>948</v>
-      </c>
-      <c r="B475" s="0" t="s">
-        <v>949</v>
-      </c>
-    </row>
-    <row r="476">
-      <c r="A476" s="0" t="s">
-        <v>950</v>
-      </c>
-      <c r="B476" s="0" t="s">
-        <v>951</v>
-      </c>
-    </row>
-    <row r="477">
-      <c r="A477" s="0" t="s">
-        <v>952</v>
-      </c>
-      <c r="B477" s="0" t="s">
-        <v>953</v>
-      </c>
-    </row>
-    <row r="478">
-      <c r="A478" s="0" t="s">
-        <v>954</v>
-      </c>
-      <c r="B478" s="0" t="s">
-        <v>955</v>
-      </c>
-    </row>
-    <row r="479">
-      <c r="A479" s="0" t="s">
-        <v>956</v>
-      </c>
-      <c r="B479" s="0" t="s">
-        <v>957</v>
-      </c>
-    </row>
-    <row r="480">
-      <c r="A480" s="0" t="s">
-        <v>958</v>
-      </c>
-      <c r="B480" s="0" t="s">
-        <v>959</v>
-      </c>
-    </row>
-    <row r="481">
-      <c r="A481" s="0" t="s">
-        <v>960</v>
-      </c>
-      <c r="B481" s="0" t="s">
-        <v>961</v>
-      </c>
-    </row>
-    <row r="482">
-      <c r="A482" s="0" t="s">
-        <v>962</v>
-      </c>
-      <c r="B482" s="0" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="483">
-      <c r="A483" s="0" t="s">
-        <v>964</v>
-      </c>
-      <c r="B483" s="0" t="s">
-        <v>965</v>
-      </c>
-    </row>
-    <row r="484">
-      <c r="A484" s="0" t="s">
-        <v>966</v>
-      </c>
-      <c r="B484" s="0" t="s">
-        <v>967</v>
-      </c>
-    </row>
-    <row r="485">
-      <c r="A485" s="0" t="s">
-        <v>968</v>
-      </c>
-      <c r="B485" s="0" t="s">
-        <v>969</v>
-      </c>
-    </row>
-    <row r="486">
-      <c r="A486" s="0" t="s">
-        <v>970</v>
-      </c>
-      <c r="B486" s="0" t="s">
-        <v>971</v>
-      </c>
-    </row>
-    <row r="487">
-      <c r="A487" s="0" t="s">
-        <v>972</v>
-      </c>
-      <c r="B487" s="0" t="s">
-        <v>973</v>
-      </c>
-    </row>
-    <row r="488">
-      <c r="A488" s="0" t="s">
-        <v>974</v>
-      </c>
-      <c r="B488" s="0" t="s">
-        <v>975</v>
-      </c>
-    </row>
-    <row r="489">
-      <c r="A489" s="0" t="s">
-        <v>976</v>
-      </c>
-      <c r="B489" s="0" t="s">
-        <v>977</v>
-      </c>
-    </row>
-    <row r="490">
-      <c r="A490" s="0" t="s">
-        <v>978</v>
-      </c>
-      <c r="B490" s="0" t="s">
-        <v>979</v>
-      </c>
-    </row>
-    <row r="491">
-      <c r="A491" s="0" t="s">
-        <v>980</v>
-      </c>
-      <c r="B491" s="0" t="s">
-        <v>981</v>
-      </c>
-    </row>
-    <row r="492">
-      <c r="A492" s="0" t="s">
-        <v>982</v>
-      </c>
-      <c r="B492" s="0" t="s">
-        <v>983</v>
-      </c>
-    </row>
-    <row r="493">
-      <c r="A493" s="0" t="s">
-        <v>984</v>
-      </c>
-      <c r="B493" s="0" t="s">
-        <v>985</v>
-      </c>
-    </row>
-    <row r="494">
-      <c r="A494" s="0" t="s">
-        <v>986</v>
-      </c>
-      <c r="B494" s="0" t="s">
-        <v>987</v>
-      </c>
-    </row>
-    <row r="495">
-      <c r="A495" s="0" t="s">
-        <v>988</v>
-      </c>
-      <c r="B495" s="0" t="s">
-        <v>989</v>
-      </c>
-    </row>
-    <row r="496">
-      <c r="A496" s="0" t="s">
-        <v>990</v>
-      </c>
-      <c r="B496" s="0" t="s">
-        <v>991</v>
-      </c>
-    </row>
-    <row r="497">
-      <c r="A497" s="0" t="s">
-        <v>992</v>
-      </c>
-      <c r="B497" s="0" t="s">
-        <v>993</v>
-      </c>
-    </row>
-    <row r="498">
-      <c r="A498" s="0" t="s">
-        <v>994</v>
-      </c>
-      <c r="B498" s="0" t="s">
-        <v>995</v>
-      </c>
-    </row>
-    <row r="499">
-      <c r="A499" s="0" t="s">
-        <v>996</v>
-      </c>
-      <c r="B499" s="0" t="s">
-        <v>997</v>
-      </c>
-    </row>
-    <row r="500">
-      <c r="A500" s="0" t="s">
-        <v>998</v>
-      </c>
-      <c r="B500" s="0" t="s">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="501">
-      <c r="A501" s="0" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B501" s="0" t="s">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="502">
-      <c r="A502" s="0" t="s">
-        <v>1002</v>
-      </c>
-      <c r="B502" s="0" t="s">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="503">
-      <c r="A503" s="0" t="s">
-        <v>1004</v>
-      </c>
-      <c r="B503" s="0" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="504">
-      <c r="A504" s="0" t="s">
-        <v>1006</v>
-      </c>
-      <c r="B504" s="0" t="s">
-        <v>1007</v>
-      </c>
-    </row>
-    <row r="505">
-      <c r="A505" s="0" t="s">
-        <v>1008</v>
-      </c>
-      <c r="B505" s="0" t="s">
-        <v>1009</v>
-      </c>
-    </row>
-    <row r="506">
-      <c r="A506" s="0" t="s">
-        <v>1010</v>
-      </c>
-      <c r="B506" s="0" t="s">
-        <v>1011</v>
-      </c>
-    </row>
-    <row r="507">
-      <c r="A507" s="0" t="s">
-        <v>1012</v>
-      </c>
-      <c r="B507" s="0" t="s">
-        <v>1013</v>
-      </c>
-    </row>
-    <row r="508">
-      <c r="A508" s="0" t="s">
-        <v>1014</v>
-      </c>
-      <c r="B508" s="0" t="s">
-        <v>1015</v>
-      </c>
-    </row>
-    <row r="509">
-      <c r="A509" s="0" t="s">
-        <v>1016</v>
-      </c>
-      <c r="B509" s="0" t="s">
-        <v>1017</v>
-      </c>
-    </row>
-    <row r="510">
-      <c r="A510" s="0" t="s">
-        <v>1018</v>
-      </c>
-      <c r="B510" s="0" t="s">
-        <v>1019</v>
-      </c>
-    </row>
-    <row r="511">
-      <c r="A511" s="0" t="s">
-        <v>1020</v>
-      </c>
-      <c r="B511" s="0" t="s">
-        <v>1021</v>
-      </c>
-    </row>
-    <row r="512">
-      <c r="A512" s="0" t="s">
-        <v>1022</v>
-      </c>
-      <c r="B512" s="0" t="s">
-        <v>1023</v>
-      </c>
-    </row>
-    <row r="513">
-      <c r="A513" s="0" t="s">
-        <v>1024</v>
-      </c>
-      <c r="B513" s="0" t="s">
-        <v>1025</v>
-      </c>
-    </row>
-    <row r="514">
-      <c r="A514" s="0" t="s">
-        <v>1026</v>
-      </c>
-      <c r="B514" s="0" t="s">
-        <v>1027</v>
-      </c>
-    </row>
-    <row r="515">
-      <c r="A515" s="0" t="s">
-        <v>1028</v>
-      </c>
-      <c r="B515" s="0" t="s">
-        <v>1029</v>
-      </c>
-    </row>
-    <row r="516">
-      <c r="A516" s="0" t="s">
-        <v>1030</v>
-      </c>
-      <c r="B516" s="0" t="s">
-        <v>1031</v>
-      </c>
-    </row>
-    <row r="517">
-      <c r="A517" s="0" t="s">
-        <v>1032</v>
-      </c>
-      <c r="B517" s="0" t="s">
-        <v>1033</v>
-      </c>
-    </row>
   </sheetData>
   <headerFooter/>
 </worksheet>

</xml_diff>